<commit_message>
changes from late Nov
</commit_message>
<xml_diff>
--- a/data/raw/checks/Peachtree Report.xlsx
+++ b/data/raw/checks/Peachtree Report.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HazTrain5\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Finance-Model\data\raw\checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDD1B87-B1AD-484D-8C86-FF5C6DCF111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21580" windowHeight="9660"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Check Register" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,21 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Check Register'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -197,7 +209,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;\-#,##0.00;* ??"/>
@@ -224,12 +236,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -284,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -316,6 +334,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,25 +619,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="16384" width="8.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -630,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -647,7 +671,7 @@
         <v>104682.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -664,7 +688,7 @@
         <v>348.75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -681,7 +705,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -698,7 +722,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -715,7 +739,7 @@
         <v>10737.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -732,7 +756,7 @@
         <v>4610.13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -749,7 +773,7 @@
         <v>2049.7199999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -766,7 +790,7 @@
         <v>313.01</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -783,7 +807,7 @@
         <v>241.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -800,7 +824,7 @@
         <v>78718.11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -817,7 +841,7 @@
         <v>95000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -834,7 +858,7 @@
         <v>-95000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -851,7 +875,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -868,7 +892,7 @@
         <v>-1038.95</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -885,7 +909,7 @@
         <v>-564.07000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
@@ -902,7 +926,7 @@
         <v>-920.44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -919,7 +943,7 @@
         <v>-104.98</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -936,7 +960,7 @@
         <v>-4637.6499999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -953,7 +977,7 @@
         <v>-12709.41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -970,7 +994,7 @@
         <v>-2100</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
@@ -987,7 +1011,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1004,7 +1028,7 @@
         <v>1038.95</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
@@ -1021,7 +1045,7 @@
         <v>564.07000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -1038,7 +1062,7 @@
         <v>1417.05</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1055,7 +1079,7 @@
         <v>104.98</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>48</v>
       </c>
@@ -1072,11 +1096,11 @@
         <v>4637.6499999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="16">
         <v>45245</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1089,7 +1113,7 @@
         <v>12709.41</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>50</v>
       </c>
@@ -1106,7 +1130,7 @@
         <v>5262</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -1123,10 +1147,10 @@
         <v>2868.22</v>
       </c>
     </row>
-    <row r="31" spans="1:5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" s="4" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
@@ -1142,7 +1166,7 @@
         <v>290718.24999999988</v>
       </c>
     </row>
-    <row r="33" spans="1:5" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>

</xml_diff>